<commit_message>
AUTHENTICATION: Update response message for authentication middleware
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -5,42 +5,30 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Barcode</t>
   </si>
   <si>
-    <t>Product name</t>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
   <si>
     <t>Supplier Code</t>
   </si>
   <si>
-    <t>Supplier Name</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>770795005596</t>
-  </si>
-  <si>
-    <t>DAN-D-PAK HẠT ĐIỀU KHÔNG MUỐI 50G/1 GÓI</t>
-  </si>
-  <si>
-    <t>C0017</t>
-  </si>
-  <si>
-    <t>CÔNG TY CỔ PHẦN THỰC PHẨM DÂN ÔN</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Unit Cost</t>
   </si>
 </sst>
 </file>
@@ -94,13 +82,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -111,27 +99,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API: new api for updating product price
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -5,30 +5,42 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Barcode</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>UOM</t>
-  </si>
-  <si>
-    <t>Department</t>
+    <t>Product name</t>
   </si>
   <si>
     <t>Supplier Code</t>
   </si>
   <si>
-    <t>Unit Cost</t>
+    <t>Supplier Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>770795005596</t>
+  </si>
+  <si>
+    <t>DAN-D-PAK HẠT ĐIỀU KHÔNG MUỐI 50G/1 GÓI</t>
+  </si>
+  <si>
+    <t>C0017</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN THỰC PHẨM DÂN ÔN</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -82,13 +94,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -99,7 +111,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API: update new customer
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truonggiangit793/Desktop/mobile-api-service/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truonggiangit793/Desktop/crm/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E7D4BC-5BB4-0845-BF12-B60987EA29F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB81D4-48CD-2840-9B64-AD061CD6238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,6 +49,9 @@
     <t>0988664383</t>
   </si>
   <si>
+    <t>VJbbNX</t>
+  </si>
+  <si>
     <t>Manager</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>0798044844</t>
   </si>
   <si>
+    <t>GPhNHj</t>
+  </si>
+  <si>
     <t>CK-HCM0323384</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t>0901544827</t>
   </si>
   <si>
+    <t>xvbOIa</t>
+  </si>
+  <si>
     <t>CK-HCM0323773</t>
   </si>
   <si>
@@ -79,6 +88,9 @@
     <t>0335663897</t>
   </si>
   <si>
+    <t>ZbQUkX</t>
+  </si>
+  <si>
     <t>CK-PT9115</t>
   </si>
   <si>
@@ -88,6 +100,9 @@
     <t>0702907154</t>
   </si>
   <si>
+    <t>leqNom</t>
+  </si>
+  <si>
     <t>CK-PT9408</t>
   </si>
   <si>
@@ -95,6 +110,9 @@
   </si>
   <si>
     <t>0389368117</t>
+  </si>
+  <si>
+    <t>icYwig</t>
   </si>
   <si>
     <t>CK-PT9493</t>
@@ -253,37 +271,19 @@
     </r>
   </si>
   <si>
-    <t>VJBBNX</t>
-  </si>
-  <si>
-    <t>GPHNHJ</t>
-  </si>
-  <si>
-    <t>XVBOLO</t>
-  </si>
-  <si>
-    <t>ZBQUKX</t>
-  </si>
-  <si>
-    <t>LEDNOM</t>
-  </si>
-  <si>
-    <t>OPLUYP</t>
-  </si>
-  <si>
-    <t>SAGBHN</t>
-  </si>
-  <si>
-    <t>HYDRTV</t>
-  </si>
-  <si>
-    <t>WSHANL</t>
-  </si>
-  <si>
-    <t>BNSALK</t>
-  </si>
-  <si>
-    <t>SBUNFK</t>
+    <t>saHVAu</t>
+  </si>
+  <si>
+    <t>HYfdiH</t>
+  </si>
+  <si>
+    <t>wshKan</t>
+  </si>
+  <si>
+    <t>BnsJhU</t>
+  </si>
+  <si>
+    <t>sBuGyF</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1526,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1565,236 +1565,236 @@
         <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>65</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API: fix account role when register
</commit_message>
<xml_diff>
--- a/tmp/tmp.xlsx
+++ b/tmp/tmp.xlsx
@@ -11,27 +11,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Barcode</t>
+    <t>User Code</t>
   </si>
   <si>
-    <t>Product Name</t>
+    <t>Fullname</t>
   </si>
   <si>
-    <t>UOM</t>
+    <t>Email</t>
   </si>
   <si>
-    <t>Department</t>
+    <t>Phone Number</t>
   </si>
   <si>
-    <t>Supplier Code</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>Unit Cost</t>
-  </si>
-  <si>
-    <t>Quantity</t>
+    <t>Role</t>
   </si>
 </sst>
 </file>
@@ -85,13 +82,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -110,9 +107,6 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>